<commit_message>
deleting whitespace from excel
</commit_message>
<xml_diff>
--- a/app/bird_data.xlsx
+++ b/app/bird_data.xlsx
@@ -58,8 +58,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">A </t>
@@ -68,8 +68,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Eurasian</t>
@@ -77,8 +77,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -87,8 +87,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">passerine</t>
@@ -96,8 +96,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> in the </t>
@@ -106,8 +106,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">genus</t>
@@ -115,8 +115,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -125,8 +125,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Acrocephalus</t>
@@ -134,8 +134,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">. The genus name Acrocephalus is from </t>
@@ -144,8 +144,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Ancient Greek</t>
@@ -153,8 +153,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> akros, "highest", and kephale, "head". It is possible that </t>
@@ -163,8 +163,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Naumann</t>
@@ -172,8 +172,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> and </t>
@@ -182,8 +182,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Naumann</t>
@@ -191,8 +191,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> thought akros meant "sharp-pointed". The specific arundinaceus is from </t>
@@ -201,8 +201,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Latin</t>
@@ -210,15 +210,15 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> and means "like a reed", from arundo, arundinis, "reed".</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Ember </t>
+    <t xml:space="preserve">Ember</t>
   </si>
   <si>
     <t xml:space="preserve">Emberiza citrinella</t>
@@ -230,8 +230,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">A </t>
@@ -240,8 +240,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">passerine</t>
@@ -249,8 +249,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -259,8 +259,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">bird</t>
@@ -268,8 +268,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> in the </t>
@@ -278,8 +278,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">bunting</t>
@@ -287,8 +287,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> family that is native to </t>
@@ -297,8 +297,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Eurasia</t>
@@ -306,8 +306,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> and has been </t>
@@ -316,8 +316,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">introduced</t>
@@ -325,8 +325,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> to New Zealand and Australia. Most European birds remain in the breeding range year-round, but the eastern </t>
@@ -335,8 +335,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">subspecies</t>
@@ -344,8 +344,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> is partially </t>
@@ -354,8 +354,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">migratory</t>
@@ -363,8 +363,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, with much of the population wintering further south. The male yellowhammer has a bright yellow head, streaked brown back, chestnut rump, and yellow under parts. </t>
@@ -383,8 +383,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">A </t>
@@ -393,8 +393,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">passerine</t>
@@ -402,8 +402,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -412,8 +412,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">bird</t>
@@ -421,8 +421,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> in the </t>
@@ -431,8 +431,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">tit</t>
@@ -440,8 +440,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> family Paridae. It is a widespread and common species throughout Europe, the </t>
@@ -450,8 +450,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Middle East</t>
@@ -459,8 +459,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, </t>
@@ -469,8 +469,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Central Asia</t>
@@ -478,8 +478,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> and east across the </t>
@@ -488,8 +488,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Palearctic</t>
@@ -497,8 +497,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> to the </t>
@@ -507,8 +507,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Amur River</t>
@@ -516,8 +516,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, south to parts of </t>
@@ -526,8 +526,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">North Africa</t>
@@ -535,8 +535,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> where it is generally resident in any sort of woodland; most great tits do not </t>
@@ -545,8 +545,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">migrate</t>
@@ -554,8 +554,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> except in extremely harsh winters.  </t>
@@ -574,8 +574,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">A common and widespread </t>
@@ -584,8 +584,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">typical warbler</t>
@@ -593,8 +593,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">. It has mainly olive-grey upperparts and pale grey underparts, and differences between the five </t>
@@ -603,8 +603,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">subspecies</t>
@@ -612,8 +612,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> are small. Both sexes have a neat coloured cap to the head, black in the male and reddish-brown in the female. The male's typical song is a rich musical warbling, often ending in a loud high-pitched crescendo. </t>
@@ -673,21 +673,21 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val=""/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
-      <name val=""/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -788,10 +788,10 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.71"/>

</xml_diff>